<commit_message>
Updated for Pandemic Jam
Updated for prompts for Pandemic Jam.
</commit_message>
<xml_diff>
--- a/HAZMAT-Pandemic Jam.xlsx
+++ b/HAZMAT-Pandemic Jam.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Creative Cloud\Creative Cloud Files\Affinity Games\HAZMAT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Creative Cloud\Creative Cloud Files\Affinity Games\hazmatgame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C273CB96-F5FE-443F-89D8-025549BBCF6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F007CB-1932-48E4-B2E0-DD5D27DF34A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26940" yWindow="1800" windowWidth="23610" windowHeight="13275" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28080" yWindow="720" windowWidth="23610" windowHeight="13275" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="53">
   <si>
     <t>CARD_TYPE</t>
   </si>
@@ -45,39 +45,9 @@
     <t>CARD_CAT</t>
   </si>
   <si>
-    <t>How could you protect others?</t>
-  </si>
-  <si>
-    <t>How could you feel more confident?</t>
-  </si>
-  <si>
-    <t>What values could you stand up for that might lose you friends?</t>
-  </si>
-  <si>
-    <t>Who could you confide in?</t>
-  </si>
-  <si>
-    <t>What could you question about yourself, but are afraid to?</t>
-  </si>
-  <si>
     <t>@CARD_QR</t>
   </si>
   <si>
-    <t>Who is someone you felt an immediate dislike for and why?</t>
-  </si>
-  <si>
-    <t>When have you felt worthless?</t>
-  </si>
-  <si>
-    <t>How do you talk to others while playing games?</t>
-  </si>
-  <si>
-    <t>When have you intentionally hurt someone?</t>
-  </si>
-  <si>
-    <t>When have you felt emotionally overwhelmed?</t>
-  </si>
-  <si>
     <t>CARD_AorF</t>
   </si>
   <si>
@@ -90,168 +60,15 @@
     <t>F</t>
   </si>
   <si>
-    <t>When have you really feared for yourself?</t>
-  </si>
-  <si>
-    <t>When have you lost control of your anger?</t>
-  </si>
-  <si>
-    <t>When have you felt like nothing really mattered?</t>
-  </si>
-  <si>
-    <t>What is something you did or said that you are ashamed of?</t>
-  </si>
-  <si>
-    <t>When have you remained silent when you shouldn't have?</t>
-  </si>
-  <si>
-    <t>When have you blamed someone for something bad that happened to them?</t>
-  </si>
-  <si>
-    <t>When have you pressured someone into doing something they did not want to do?</t>
-  </si>
-  <si>
     <t>HAZARDOUS SITE</t>
   </si>
   <si>
     <t>HAZMAT SUIT</t>
   </si>
   <si>
-    <t>Who could you ask for help?</t>
-  </si>
-  <si>
-    <t>How could you better understand what someone else is experiencing?</t>
-  </si>
-  <si>
-    <t>How could you show that you respect someone?</t>
-  </si>
-  <si>
-    <t>How could you support someone?</t>
-  </si>
-  <si>
-    <t>How could you stand up for someone?</t>
-  </si>
-  <si>
     <t>HAZARDOUS MATERIALS</t>
   </si>
   <si>
-    <t>When have you used a slur and why?</t>
-  </si>
-  <si>
-    <t>When have you viewed another person as a means to an end?</t>
-  </si>
-  <si>
-    <t>When have you used another person for selfish reasons?</t>
-  </si>
-  <si>
-    <t>When was winning more important than how you won?</t>
-  </si>
-  <si>
-    <t>A friend calls someone you know a "Fag!" in front of you…</t>
-  </si>
-  <si>
-    <t>You are intoxicated...</t>
-  </si>
-  <si>
-    <t>You see your friends picking a fight with someone...</t>
-  </si>
-  <si>
-    <t>Someone is trying to pick a fight with you...</t>
-  </si>
-  <si>
-    <t>You see your friend threatening someone...</t>
-  </si>
-  <si>
-    <t>A friend says they have been "Friend Zoned" by someone they are attracted to...</t>
-  </si>
-  <si>
-    <t>You have moved somewhere new and are trying to make new friends...</t>
-  </si>
-  <si>
-    <t>Someone has called you a "Pussy!" in front of your friends...</t>
-  </si>
-  <si>
-    <t>You see a friend grope someone...</t>
-  </si>
-  <si>
-    <t>You are trying to seduce someone...</t>
-  </si>
-  <si>
-    <t>How could you de-escalate a situation?</t>
-  </si>
-  <si>
-    <t>How could you get to know someone different from yourself?</t>
-  </si>
-  <si>
-    <t>When have you criticized something or someone as "girly" or "gay"?</t>
-  </si>
-  <si>
-    <t>What is a difficult criticism you have received?</t>
-  </si>
-  <si>
-    <t>What is a deeply painful thing you have experienced?</t>
-  </si>
-  <si>
-    <t>How does holding a weapon make you feel?</t>
-  </si>
-  <si>
-    <t>How could you become a better person?</t>
-  </si>
-  <si>
-    <t>How could you make a positive impact?</t>
-  </si>
-  <si>
-    <t>You have been rejected...</t>
-  </si>
-  <si>
-    <t>What is a bad decision you made when intoxicated?</t>
-  </si>
-  <si>
-    <t>What is something you have done that you could get in trouble for?</t>
-  </si>
-  <si>
-    <t>When have you felt humiliated?</t>
-  </si>
-  <si>
-    <t>How have you publicly embarased someone?</t>
-  </si>
-  <si>
-    <t>When have you felt jealous and why?</t>
-  </si>
-  <si>
-    <t>When have you felt alone and why?</t>
-  </si>
-  <si>
-    <t>What is a conspiracy that you have believed in and why?</t>
-  </si>
-  <si>
-    <t>How have you badgered or bullied someone and why?</t>
-  </si>
-  <si>
-    <t>When have you shut down a conversation and why?</t>
-  </si>
-  <si>
-    <t>Who is someone you felt contempt for and why?</t>
-  </si>
-  <si>
-    <t>What is a bad decision you made and why?</t>
-  </si>
-  <si>
-    <t>When have you plotted revenge and why?</t>
-  </si>
-  <si>
-    <t>When have you acted violently and why?</t>
-  </si>
-  <si>
-    <t>When have you excluded someone and why?</t>
-  </si>
-  <si>
-    <t>When have you neglected a responsibility and why?</t>
-  </si>
-  <si>
-    <t>How have you made someone feel uncomfortable (intentionally or otherwise)?</t>
-  </si>
-  <si>
     <t>FLAMMABLE</t>
   </si>
   <si>
@@ -324,31 +141,49 @@
     <t>Hazardous-Material.ai</t>
   </si>
   <si>
-    <t>Your friends have embarrassed you in front of other people...</t>
-  </si>
-  <si>
-    <t>How could you communicate better?</t>
-  </si>
-  <si>
-    <t>You hear a friend use a slur...</t>
-  </si>
-  <si>
-    <t>A friend of yours has been accused of sexual assault by someone...</t>
-  </si>
-  <si>
-    <t>You are thinking about harming yourself...</t>
-  </si>
-  <si>
-    <t>What was a difficult rejection you received and why?</t>
-  </si>
-  <si>
-    <t>When have you not cared when you should have and why?</t>
-  </si>
-  <si>
-    <t>How has porn affected how you think about sex?</t>
-  </si>
-  <si>
-    <t>What do you think you are owed and why?</t>
+    <t>You are going to the grocery store...</t>
+  </si>
+  <si>
+    <t>You have lost your job...</t>
+  </si>
+  <si>
+    <t>You have tested positive...</t>
+  </si>
+  <si>
+    <t>You have developed a cough...</t>
+  </si>
+  <si>
+    <t>You have developed a fever...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How have you been physically distancing yourself? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">How have you overestimated your health resilience? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">When did you take a risk you knew you should not have? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">How have you talked to your family about the risks and precautions? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">How have you shared misinformation (knowingly or otherwise)? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">How could you help your neighbors? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">How could you support someone who has lost their job? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">How could you protect others? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">How could you socialize safely right now? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">How could you date safely right now? </t>
   </si>
 </sst>
 </file>
@@ -680,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37:E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,7 +539,7 @@
         <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -716,87 +551,87 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>83</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F2" t="s">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="G2" t="s">
-        <v>96</v>
+        <v>35</v>
       </c>
       <c r="H2" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>99</v>
+        <v>39</v>
       </c>
       <c r="F3" t="s">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="G3" t="s">
-        <v>96</v>
+        <v>35</v>
       </c>
       <c r="H3" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="F4" t="s">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="G4" t="s">
-        <v>96</v>
+        <v>35</v>
       </c>
       <c r="H4" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
         <v>4</v>
@@ -805,1696 +640,1535 @@
         <v>41</v>
       </c>
       <c r="F5" t="s">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="G5" t="s">
-        <v>96</v>
+        <v>35</v>
       </c>
       <c r="H5" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F6" t="s">
-        <v>93</v>
+        <v>32</v>
       </c>
       <c r="G6" t="s">
-        <v>96</v>
+        <v>35</v>
       </c>
       <c r="H6" t="s">
-        <v>76</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
       </c>
-      <c r="E7" t="s">
-        <v>43</v>
-      </c>
       <c r="F7" t="s">
-        <v>93</v>
+        <v>32</v>
       </c>
       <c r="G7" t="s">
-        <v>96</v>
+        <v>35</v>
       </c>
       <c r="H7" t="s">
-        <v>76</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>80</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
         <v>4</v>
       </c>
-      <c r="E8" t="s">
-        <v>44</v>
-      </c>
       <c r="F8" t="s">
-        <v>93</v>
+        <v>32</v>
       </c>
       <c r="G8" t="s">
-        <v>96</v>
+        <v>35</v>
       </c>
       <c r="H8" t="s">
-        <v>76</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>80</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
         <v>4</v>
       </c>
-      <c r="E9" t="s">
-        <v>103</v>
-      </c>
       <c r="F9" t="s">
-        <v>93</v>
+        <v>32</v>
       </c>
       <c r="G9" t="s">
-        <v>96</v>
+        <v>35</v>
       </c>
       <c r="H9" t="s">
-        <v>76</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>81</v>
+        <v>20</v>
       </c>
       <c r="D10" t="s">
         <v>4</v>
       </c>
-      <c r="E10" t="s">
-        <v>45</v>
-      </c>
       <c r="F10" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="G10" t="s">
-        <v>96</v>
+        <v>35</v>
       </c>
       <c r="H10" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>81</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
         <v>4</v>
       </c>
-      <c r="E11" t="s">
-        <v>46</v>
-      </c>
       <c r="F11" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="G11" t="s">
-        <v>96</v>
+        <v>35</v>
       </c>
       <c r="H11" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>81</v>
+        <v>20</v>
       </c>
       <c r="D12" t="s">
         <v>4</v>
       </c>
-      <c r="E12" t="s">
-        <v>47</v>
-      </c>
       <c r="F12" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="G12" t="s">
-        <v>96</v>
+        <v>35</v>
       </c>
       <c r="H12" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>81</v>
+        <v>20</v>
       </c>
       <c r="D13" t="s">
         <v>4</v>
       </c>
-      <c r="E13" t="s">
-        <v>101</v>
-      </c>
       <c r="F13" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="G13" t="s">
-        <v>96</v>
+        <v>35</v>
       </c>
       <c r="H13" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>82</v>
+        <v>21</v>
       </c>
       <c r="D14" t="s">
         <v>4</v>
       </c>
-      <c r="E14" t="s">
-        <v>48</v>
-      </c>
       <c r="F14" t="s">
-        <v>95</v>
+        <v>34</v>
       </c>
       <c r="G14" t="s">
-        <v>96</v>
+        <v>35</v>
       </c>
       <c r="H14" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>82</v>
+        <v>21</v>
       </c>
       <c r="D15" t="s">
         <v>4</v>
       </c>
-      <c r="E15" t="s">
-        <v>102</v>
-      </c>
       <c r="F15" t="s">
-        <v>95</v>
+        <v>34</v>
       </c>
       <c r="G15" t="s">
-        <v>96</v>
+        <v>35</v>
       </c>
       <c r="H15" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>82</v>
+        <v>21</v>
       </c>
       <c r="D16" t="s">
         <v>4</v>
       </c>
-      <c r="E16" t="s">
-        <v>49</v>
-      </c>
       <c r="F16" t="s">
-        <v>95</v>
+        <v>34</v>
       </c>
       <c r="G16" t="s">
-        <v>96</v>
+        <v>35</v>
       </c>
       <c r="H16" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D17" t="s">
         <v>4</v>
       </c>
       <c r="E17" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F17" t="s">
-        <v>88</v>
+        <v>27</v>
       </c>
       <c r="G17" t="s">
-        <v>97</v>
+        <v>36</v>
       </c>
       <c r="H17" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D18" t="s">
         <v>4</v>
       </c>
       <c r="E18" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="F18" t="s">
-        <v>88</v>
+        <v>27</v>
       </c>
       <c r="G18" t="s">
-        <v>97</v>
+        <v>36</v>
       </c>
       <c r="H18" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D19" t="s">
         <v>4</v>
       </c>
       <c r="E19" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="F19" t="s">
-        <v>88</v>
+        <v>27</v>
       </c>
       <c r="G19" t="s">
-        <v>97</v>
+        <v>36</v>
       </c>
       <c r="H19" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D20" t="s">
         <v>4</v>
       </c>
       <c r="E20" t="s">
-        <v>100</v>
+        <v>51</v>
       </c>
       <c r="F20" t="s">
-        <v>88</v>
+        <v>27</v>
       </c>
       <c r="G20" t="s">
-        <v>97</v>
+        <v>36</v>
       </c>
       <c r="H20" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D21" t="s">
         <v>4</v>
       </c>
       <c r="E21" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="F21" t="s">
-        <v>89</v>
+        <v>28</v>
       </c>
       <c r="G21" t="s">
-        <v>97</v>
+        <v>36</v>
       </c>
       <c r="H21" t="s">
-        <v>76</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D22" t="s">
         <v>4</v>
       </c>
-      <c r="E22" t="s">
-        <v>6</v>
-      </c>
       <c r="F22" t="s">
-        <v>89</v>
+        <v>28</v>
       </c>
       <c r="G22" t="s">
-        <v>97</v>
+        <v>36</v>
       </c>
       <c r="H22" t="s">
-        <v>76</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D23" t="s">
         <v>4</v>
       </c>
-      <c r="E23" t="s">
-        <v>50</v>
-      </c>
       <c r="F23" t="s">
-        <v>89</v>
+        <v>28</v>
       </c>
       <c r="G23" t="s">
-        <v>97</v>
+        <v>36</v>
       </c>
       <c r="H23" t="s">
-        <v>76</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" t="s">
         <v>29</v>
       </c>
-      <c r="B24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" t="s">
-        <v>4</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F24" t="s">
-        <v>90</v>
-      </c>
       <c r="G24" t="s">
-        <v>97</v>
+        <v>36</v>
       </c>
       <c r="H24" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" t="s">
         <v>29</v>
       </c>
-      <c r="B25" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" t="s">
-        <v>4</v>
-      </c>
-      <c r="E25" t="s">
-        <v>8</v>
-      </c>
-      <c r="F25" t="s">
-        <v>90</v>
-      </c>
       <c r="G25" t="s">
-        <v>97</v>
+        <v>36</v>
       </c>
       <c r="H25" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" t="s">
         <v>29</v>
       </c>
-      <c r="B26" t="s">
-        <v>29</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D26" t="s">
-        <v>4</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F26" t="s">
-        <v>90</v>
-      </c>
       <c r="G26" t="s">
-        <v>97</v>
+        <v>36</v>
       </c>
       <c r="H26" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" t="s">
         <v>29</v>
       </c>
-      <c r="B27" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" t="s">
-        <v>4</v>
-      </c>
-      <c r="E27" t="s">
-        <v>51</v>
-      </c>
-      <c r="F27" t="s">
-        <v>90</v>
-      </c>
       <c r="G27" t="s">
-        <v>97</v>
+        <v>36</v>
       </c>
       <c r="H27" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D28" t="s">
         <v>4</v>
       </c>
-      <c r="E28" t="s">
-        <v>9</v>
-      </c>
       <c r="F28" t="s">
-        <v>91</v>
+        <v>30</v>
       </c>
       <c r="G28" t="s">
-        <v>97</v>
+        <v>36</v>
       </c>
       <c r="H28" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D29" t="s">
         <v>4</v>
       </c>
-      <c r="E29" t="s">
-        <v>10</v>
-      </c>
       <c r="F29" t="s">
-        <v>91</v>
+        <v>30</v>
       </c>
       <c r="G29" t="s">
-        <v>97</v>
+        <v>36</v>
       </c>
       <c r="H29" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D30" t="s">
         <v>4</v>
       </c>
-      <c r="E30" t="s">
-        <v>31</v>
-      </c>
       <c r="F30" t="s">
-        <v>91</v>
+        <v>30</v>
       </c>
       <c r="G30" t="s">
-        <v>97</v>
+        <v>36</v>
       </c>
       <c r="H30" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="B31" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D31" t="s">
         <v>4</v>
       </c>
-      <c r="E31" t="s">
-        <v>32</v>
-      </c>
       <c r="F31" t="s">
-        <v>91</v>
+        <v>30</v>
       </c>
       <c r="G31" t="s">
-        <v>97</v>
+        <v>36</v>
       </c>
       <c r="H31" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B32" t="s">
-        <v>84</v>
+        <v>23</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D32" t="s">
         <v>4</v>
       </c>
       <c r="E32" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="F32" t="s">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="G32" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="H32" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B33" t="s">
-        <v>84</v>
+        <v>23</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D33" t="s">
         <v>4</v>
       </c>
       <c r="E33" t="s">
+        <v>44</v>
+      </c>
+      <c r="F33" t="s">
+        <v>31</v>
+      </c>
+      <c r="G33" t="s">
+        <v>37</v>
+      </c>
+      <c r="H33" t="s">
         <v>14</v>
-      </c>
-      <c r="F33" t="s">
-        <v>92</v>
-      </c>
-      <c r="G33" t="s">
-        <v>98</v>
-      </c>
-      <c r="H33" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B34" t="s">
-        <v>84</v>
+        <v>23</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D34" t="s">
         <v>4</v>
       </c>
       <c r="E34" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="F34" t="s">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="G34" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="H34" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B35" t="s">
-        <v>84</v>
+        <v>23</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D35" t="s">
         <v>4</v>
       </c>
       <c r="E35" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="F35" t="s">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="G35" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="H35" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B36" t="s">
-        <v>84</v>
+        <v>23</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D36" t="s">
         <v>4</v>
       </c>
       <c r="E36" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="F36" t="s">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="G36" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="H36" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B37" t="s">
-        <v>84</v>
+        <v>23</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D37" t="s">
         <v>4</v>
       </c>
-      <c r="E37" t="s">
-        <v>54</v>
-      </c>
       <c r="F37" t="s">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="G37" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="H37" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B38" t="s">
-        <v>84</v>
+        <v>23</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D38" t="s">
         <v>4</v>
       </c>
-      <c r="E38" t="s">
-        <v>12</v>
-      </c>
       <c r="F38" t="s">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="G38" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="H38" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B39" t="s">
-        <v>84</v>
+        <v>23</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D39" t="s">
         <v>4</v>
       </c>
-      <c r="E39" t="s">
-        <v>53</v>
-      </c>
       <c r="F39" t="s">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="G39" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="H39" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B40" t="s">
-        <v>84</v>
+        <v>23</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D40" t="s">
         <v>4</v>
       </c>
-      <c r="E40" t="s">
-        <v>13</v>
-      </c>
       <c r="F40" t="s">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="G40" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="H40" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B41" t="s">
-        <v>84</v>
+        <v>23</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D41" t="s">
         <v>4</v>
       </c>
-      <c r="E41" t="s">
-        <v>104</v>
-      </c>
       <c r="F41" t="s">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="G41" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="H41" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B42" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D42" t="s">
         <v>4</v>
       </c>
-      <c r="E42" t="s">
-        <v>70</v>
-      </c>
       <c r="F42" t="s">
-        <v>93</v>
+        <v>32</v>
       </c>
       <c r="G42" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="H42" t="s">
-        <v>76</v>
+        <v>15</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B43" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D43" t="s">
         <v>4</v>
       </c>
-      <c r="E43" t="s">
-        <v>62</v>
-      </c>
       <c r="F43" t="s">
-        <v>93</v>
+        <v>32</v>
       </c>
       <c r="G43" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="H43" t="s">
-        <v>76</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B44" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D44" t="s">
         <v>4</v>
       </c>
-      <c r="E44" t="s">
-        <v>60</v>
-      </c>
       <c r="F44" t="s">
-        <v>93</v>
+        <v>32</v>
       </c>
       <c r="G44" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="H44" t="s">
-        <v>76</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B45" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D45" t="s">
         <v>4</v>
       </c>
-      <c r="E45" t="s">
-        <v>71</v>
-      </c>
       <c r="F45" t="s">
-        <v>93</v>
+        <v>32</v>
       </c>
       <c r="G45" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="H45" t="s">
-        <v>76</v>
+        <v>15</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B46" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D46" t="s">
         <v>4</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
+        <v>32</v>
+      </c>
+      <c r="G46" t="s">
+        <v>37</v>
+      </c>
+      <c r="H46" t="s">
         <v>15</v>
-      </c>
-      <c r="F46" t="s">
-        <v>93</v>
-      </c>
-      <c r="G46" t="s">
-        <v>98</v>
-      </c>
-      <c r="H46" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B47" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D47" t="s">
         <v>4</v>
       </c>
-      <c r="E47" t="s">
-        <v>22</v>
-      </c>
       <c r="F47" t="s">
-        <v>93</v>
+        <v>32</v>
       </c>
       <c r="G47" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="H47" t="s">
-        <v>76</v>
+        <v>15</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B48" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D48" t="s">
         <v>4</v>
       </c>
-      <c r="E48" t="s">
-        <v>16</v>
-      </c>
       <c r="F48" t="s">
-        <v>93</v>
+        <v>32</v>
       </c>
       <c r="G48" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="H48" t="s">
-        <v>76</v>
+        <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B49" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D49" t="s">
         <v>4</v>
       </c>
-      <c r="E49" t="s">
-        <v>21</v>
-      </c>
       <c r="F49" t="s">
-        <v>93</v>
+        <v>32</v>
       </c>
       <c r="G49" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="H49" t="s">
-        <v>76</v>
+        <v>15</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B50" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D50" t="s">
         <v>4</v>
       </c>
-      <c r="E50" t="s">
-        <v>55</v>
-      </c>
       <c r="F50" t="s">
-        <v>93</v>
+        <v>32</v>
       </c>
       <c r="G50" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="H50" t="s">
-        <v>76</v>
+        <v>15</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B51" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D51" t="s">
         <v>4</v>
       </c>
-      <c r="E51" s="4" t="s">
-        <v>61</v>
-      </c>
+      <c r="E51" s="4"/>
       <c r="F51" t="s">
-        <v>93</v>
+        <v>32</v>
       </c>
       <c r="G51" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="H51" t="s">
-        <v>76</v>
+        <v>15</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B52" t="s">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D52" t="s">
         <v>4</v>
       </c>
-      <c r="E52" t="s">
-        <v>105</v>
-      </c>
       <c r="F52" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="G52" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="H52" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B53" t="s">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D53" t="s">
         <v>4</v>
       </c>
-      <c r="E53" t="s">
-        <v>24</v>
-      </c>
       <c r="F53" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="G53" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="H53" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B54" t="s">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D54" t="s">
         <v>4</v>
       </c>
-      <c r="E54" t="s">
-        <v>36</v>
-      </c>
       <c r="F54" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="G54" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="H54" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B55" t="s">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D55" t="s">
         <v>4</v>
       </c>
-      <c r="E55" t="s">
-        <v>72</v>
-      </c>
       <c r="F55" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="G55" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="H55" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B56" t="s">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D56" t="s">
         <v>4</v>
       </c>
-      <c r="E56" t="s">
-        <v>73</v>
-      </c>
       <c r="F56" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="G56" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="H56" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B57" t="s">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D57" t="s">
         <v>4</v>
       </c>
-      <c r="E57" t="s">
-        <v>25</v>
-      </c>
       <c r="F57" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="G57" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="H57" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B58" t="s">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D58" t="s">
         <v>4</v>
       </c>
-      <c r="E58" t="s">
-        <v>52</v>
-      </c>
       <c r="F58" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="G58" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="H58" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B59" t="s">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D59" t="s">
         <v>4</v>
       </c>
-      <c r="E59" s="3" t="s">
-        <v>74</v>
-      </c>
+      <c r="E59" s="3"/>
       <c r="F59" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="G59" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="H59" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B60" t="s">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D60" t="s">
         <v>4</v>
       </c>
-      <c r="E60" t="s">
-        <v>64</v>
-      </c>
       <c r="F60" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="G60" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="H60" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B61" t="s">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D61" t="s">
         <v>4</v>
       </c>
-      <c r="E61" t="s">
-        <v>106</v>
-      </c>
       <c r="F61" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="G61" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="H61" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B62" t="s">
-        <v>87</v>
+        <v>26</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D62" t="s">
         <v>4</v>
       </c>
-      <c r="E62" t="s">
-        <v>23</v>
-      </c>
       <c r="F62" t="s">
-        <v>95</v>
+        <v>34</v>
       </c>
       <c r="G62" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="H62" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B63" t="s">
-        <v>87</v>
+        <v>26</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D63" t="s">
         <v>4</v>
       </c>
-      <c r="E63" t="s">
-        <v>65</v>
-      </c>
       <c r="F63" t="s">
-        <v>95</v>
+        <v>34</v>
       </c>
       <c r="G63" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="H63" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B64" t="s">
-        <v>87</v>
+        <v>26</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D64" t="s">
         <v>4</v>
       </c>
-      <c r="E64" t="s">
-        <v>26</v>
-      </c>
       <c r="F64" t="s">
-        <v>95</v>
+        <v>34</v>
       </c>
       <c r="G64" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="H64" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B65" t="s">
-        <v>87</v>
+        <v>26</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D65" t="s">
         <v>4</v>
       </c>
-      <c r="E65" t="s">
-        <v>66</v>
-      </c>
       <c r="F65" t="s">
-        <v>95</v>
+        <v>34</v>
       </c>
       <c r="G65" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="H65" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B66" t="s">
-        <v>87</v>
+        <v>26</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D66" t="s">
         <v>4</v>
       </c>
-      <c r="E66" t="s">
-        <v>27</v>
-      </c>
       <c r="F66" t="s">
-        <v>95</v>
+        <v>34</v>
       </c>
       <c r="G66" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="H66" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B67" t="s">
-        <v>87</v>
+        <v>26</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D67" t="s">
         <v>4</v>
       </c>
-      <c r="E67" t="s">
-        <v>67</v>
-      </c>
       <c r="F67" t="s">
-        <v>95</v>
+        <v>34</v>
       </c>
       <c r="G67" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="H67" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B68" t="s">
-        <v>87</v>
+        <v>26</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D68" t="s">
         <v>4</v>
       </c>
-      <c r="E68" t="s">
-        <v>38</v>
-      </c>
       <c r="F68" t="s">
-        <v>95</v>
+        <v>34</v>
       </c>
       <c r="G68" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="H68" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B69" t="s">
-        <v>87</v>
+        <v>26</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D69" t="s">
         <v>4</v>
       </c>
-      <c r="E69" t="s">
-        <v>68</v>
-      </c>
       <c r="F69" t="s">
-        <v>95</v>
+        <v>34</v>
       </c>
       <c r="G69" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="H69" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B70" t="s">
-        <v>87</v>
+        <v>26</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D70" t="s">
         <v>4</v>
       </c>
-      <c r="E70" t="s">
-        <v>107</v>
-      </c>
       <c r="F70" t="s">
-        <v>95</v>
+        <v>34</v>
       </c>
       <c r="G70" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="H70" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B71" t="s">
-        <v>87</v>
+        <v>26</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D71" t="s">
         <v>4</v>
       </c>
-      <c r="E71" t="s">
-        <v>37</v>
-      </c>
       <c r="F71" t="s">
-        <v>95</v>
+        <v>34</v>
       </c>
       <c r="G71" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="H71" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>